<commit_message>
user register process, hand successfully, waiting for verify code finishend
</commit_message>
<xml_diff>
--- a/数据库设计.xlsx
+++ b/数据库设计.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1822A82A-FD76-404C-AD9E-46333DEA1CDC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB4BE05-E811-4E3E-9236-4637491BEC8D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO" sheetId="1" r:id="rId1"/>
     <sheet name="wxadmin" sheetId="2" r:id="rId2"/>
     <sheet name="msgcount" sheetId="3" r:id="rId3"/>
+    <sheet name="wxuser" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,18 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>wxcount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>smscount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>emailcount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>修改</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -164,6 +153,50 @@
   </si>
   <si>
     <t>memo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 首先从wxadmin表中查询出来该公司id对应的管理员的wxid（微信账号）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 如果没有这个公司id，或者enable未0，提示用户管理员还未注册，该公司账号还没有生效，并结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>step</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 查询是否这个wxid已经注册过，在当前这个wxuser表中是否有这个用户和公司对应的id，并且是active=1，step=9的，如果有有就是注册过，提示已注册，并结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. 请这个微信用户找管理员要这个注册码，如果输入正确，则账号激活，step设置成9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 如果查出来active等于1，并且step=1，则该用户在等待注册码，跳转至输入注册码页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.  如果这个用户未注册，在wxadmin中查询这个公司id及购买的userlimit的总数，没有超过poinfo的规定限制，跳转至用户输入信息的页面，点击提交把用户填写的信息保存在表里面，并把注册码保存在本表中，把step设置成1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 跳转至等待输入注册码的页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 给管理员的微信发送一个模板消息，模板消息中带有随机生成的注册码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条件是wxid存在，且active=1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -664,12 +697,12 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.15">
@@ -698,7 +731,7 @@
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
         <v>21</v>
@@ -753,13 +786,14 @@
   <dimension ref="B3:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.15">
@@ -792,13 +826,13 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.15">
@@ -822,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -840,13 +874,13 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
@@ -857,6 +891,116 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFEC9C2-59D3-4172-A8AB-D55259EE2CB2}">
+  <dimension ref="B4:L30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>